<commit_message>
Finished the presentation slides.
</commit_message>
<xml_diff>
--- a/planeamento/Planeamento-Detalhado.xlsx
+++ b/planeamento/Planeamento-Detalhado.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="95">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t xml:space="preserve">Apresentação de projetos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exame 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exame 2</t>
   </si>
   <si>
     <t xml:space="preserve">Professor</t>
@@ -306,9 +312,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -454,7 +462,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,6 +525,18 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -632,10 +652,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -935,6 +955,28 @@
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="n">
+        <v>43467</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="18" t="n">
+        <v>0.479166666666667</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16" t="n">
+        <v>43501</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="18" t="n">
+        <v>0.479166666666667</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="26">
@@ -992,7 +1034,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="16" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -1000,377 +1042,377 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>40</v>
+      <c r="E1" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22" t="s">
-        <v>42</v>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22" t="s">
-        <v>42</v>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="20" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>64</v>
+      <c r="A12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>67</v>
+      <c r="A13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>69</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22" t="s">
-        <v>42</v>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>69</v>
+      <c r="A14" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>42</v>
+        <v>73</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>73</v>
+      <c r="A15" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>75</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="22" t="s">
-        <v>47</v>
+      <c r="E15" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>75</v>
+      <c r="A16" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>77</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22" t="s">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22" t="s">
-        <v>47</v>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22" t="s">
-        <v>47</v>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22" t="s">
-        <v>42</v>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22" t="s">
-        <v>47</v>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>82</v>
+      <c r="A21" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22" t="s">
-        <v>47</v>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="A22" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22" t="s">
-        <v>47</v>
+        <v>86</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>51</v>
+      <c r="A23" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="20" t="s">
+      <c r="A24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>42</v>
+        <v>89</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>51</v>
+      <c r="A25" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="22"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>90</v>
+      <c r="A26" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22" t="s">
-        <v>47</v>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>92</v>
+      <c r="A27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22" t="s">
-        <v>42</v>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Baum-Welch algorithm.
</commit_message>
<xml_diff>
--- a/planeamento/Planeamento-Detalhado.xlsx
+++ b/planeamento/Planeamento-Detalhado.xlsx
@@ -461,7 +461,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,7 +482,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,8 +498,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -507,6 +511,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -654,7 +666,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,7 +721,7 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="7"/>
@@ -719,7 +731,7 @@
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -730,17 +742,17 @@
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +763,7 @@
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="7"/>
@@ -761,7 +773,7 @@
       <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +784,7 @@
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="7"/>
@@ -782,7 +794,7 @@
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,7 +802,7 @@
         <f aca="false">A10+7</f>
         <v>43395</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -800,7 +812,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="6"/>
@@ -811,28 +823,28 @@
         <f aca="false">A12+7</f>
         <v>43402</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
         <f aca="false">A14+7</f>
         <v>43409</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -842,7 +854,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="6"/>
@@ -853,7 +865,7 @@
         <f aca="false">A16+7</f>
         <v>43416</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -863,7 +875,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="6"/>
@@ -874,7 +886,7 @@
         <f aca="false">A18+7</f>
         <v>43423</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -884,7 +896,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="6"/>
@@ -895,7 +907,7 @@
         <f aca="false">A20+7</f>
         <v>43430</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -905,7 +917,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="6"/>
@@ -916,7 +928,7 @@
         <f aca="false">A22+7</f>
         <v>43437</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -928,7 +940,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="6"/>
@@ -939,41 +951,41 @@
         <f aca="false">A24+7</f>
         <v>43444</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="n">
+      <c r="A29" s="19" t="n">
         <v>43473</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="18" t="n">
+      <c r="C29" s="21" t="n">
         <v>0.479166666666667</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="n">
+      <c r="A30" s="19" t="n">
         <v>43501</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="18" t="n">
+      <c r="C30" s="21" t="n">
         <v>0.333333333333333</v>
       </c>
     </row>
@@ -1033,7 +1045,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -1041,376 +1053,376 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="27"/>
+      <c r="E7" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="26" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="27"/>
+      <c r="E9" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="26" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="27"/>
+      <c r="E11" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="26" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="25" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25" t="s">
+      <c r="D17" s="27"/>
+      <c r="E17" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25" t="s">
+      <c r="D18" s="27"/>
+      <c r="E18" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25" t="s">
+      <c r="D20" s="27"/>
+      <c r="E20" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>84</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25" t="s">
+      <c r="D21" s="27"/>
+      <c r="E21" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25" t="s">
+      <c r="D22" s="27"/>
+      <c r="E22" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="28" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="25"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="26" t="s">
         <v>92</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25" t="s">
+      <c r="D26" s="27"/>
+      <c r="E26" s="28" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="26" t="s">
         <v>94</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25" t="s">
+      <c r="D27" s="27"/>
+      <c r="E27" s="28" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added slides for indexin, querying and distributed IR.
</commit_message>
<xml_diff>
--- a/planeamento/Planeamento-Detalhado.xlsx
+++ b/planeamento/Planeamento-Detalhado.xlsx
@@ -474,7 +474,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -571,40 +571,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -739,7 +735,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -948,7 +944,7 @@
     </row>
     <row r="19" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="19"/>
@@ -959,20 +955,20 @@
         <f aca="false">A18+7</f>
         <v>43423</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15"/>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="14"/>
     </row>
     <row r="22" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +976,7 @@
         <f aca="false">A20+7</f>
         <v>43430</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -990,7 +986,7 @@
     </row>
     <row r="23" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9"/>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="6"/>
@@ -1001,64 +997,64 @@
         <f aca="false">A22+7</f>
         <v>43437</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15"/>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <f aca="false">A24+7</f>
         <v>43444</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="33" t="n">
+      <c r="A29" s="32" t="n">
         <v>43473</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="35" t="n">
+      <c r="C29" s="34" t="n">
         <v>0.479166666666667</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="33" t="n">
+      <c r="A30" s="32" t="n">
         <v>43501</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="35" t="n">
+      <c r="C30" s="34" t="n">
         <v>0.333333333333333</v>
       </c>
     </row>
@@ -1118,7 +1114,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="54.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="35" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
@@ -1126,376 +1122,376 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42" t="s">
+      <c r="C13" s="27"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="42" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42" t="s">
+      <c r="D18" s="40"/>
+      <c r="E18" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42" t="s">
+      <c r="D20" s="40"/>
+      <c r="E20" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42" t="s">
+      <c r="C21" s="27"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42" t="s">
+      <c r="D22" s="40"/>
+      <c r="E22" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="42"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="42"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="42" t="s">
+      <c r="D26" s="40"/>
+      <c r="E26" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="42" t="s">
+      <c r="C27" s="27"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="41" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>